<commit_message>
Some additional work - Nothing pretty new
</commit_message>
<xml_diff>
--- a/Code/Data/RVq.xlsx
+++ b/Code/Data/RVq.xlsx
@@ -346,1372 +346,1372 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1454.5965694933464</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1534.6040116000097</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1464.2849965266778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1688.037161293342</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2163.6133543200117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1985.1303548266769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2158.4372914066748</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2270.4529237266756</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2464.3458607000098</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2778.287276266678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2503.7781473333416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3218.3736684266755</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2876.8409442400093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2806.9899713866762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2292.1010221333422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3108.2565573733432</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3945.8160293266769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5092.6851591600089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6252.4970019933535</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>9036.006329806698</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10155.626413433363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>14364.7966274667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>15742.704280193362</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>17167.973299466688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>21466.529209340035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>21257.231542420031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>18695.367390206698</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>17065.491231306685</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>18738.112270566689</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>20722.301095753373</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>14006.765644880032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>13100.530956033364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>15011.748791753367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>19125.846211693355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>24326.467555626699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>30181.355521253357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35159.489554966691</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>38059.285705226685</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>33843.244337953365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>35575.772672986692</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>32159.614807153357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>34502.91515248669</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>29763.732515826694</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>37678.012508300031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>50681.003006573417</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>51859.662912626773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>54549.964382153434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>58235.876947853445</v>
+        <v>4.3842282610692326E-4</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>54618.430731913446</v>
+        <v>5.7635459221792402E-3</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>34878.475148140024</v>
+        <v>3.4742413835288353E-3</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>34969.028479260021</v>
+        <v>3.423846440254862E-3</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>45960.119072986745</v>
+        <v>1.1769097214180059E-3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>56433.157456473426</v>
+        <v>5.266672963978406E-4</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>59520.043605666782</v>
+        <v>6.0297968775836666E-4</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>62748.535101106769</v>
+        <v>1.5322466184284026E-3</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>70531.559339253421</v>
+        <v>2.6489129979985644E-4</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>82574.068680646757</v>
+        <v>2.8912988887455242E-4</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>88885.743152753435</v>
+        <v>6.0971688173581744E-4</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>92580.239427686742</v>
+        <v>2.9007766401845087E-4</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>95437.249260486758</v>
+        <v>4.4148067889388502E-4</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>105598.43432042013</v>
+        <v>3.3081102379655964E-4</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>99532.419807900107</v>
+        <v>1.0325217359824781E-3</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>110655.56899270677</v>
+        <v>3.3849844641362542E-4</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>116785.78963581345</v>
+        <v>4.2932739999858782E-4</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>108278.77026958675</v>
+        <v>1.5141453322527389E-3</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>96151.227939666758</v>
+        <v>1.807267658398972E-3</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>76612.081908366788</v>
+        <v>2.3498565942443213E-3</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>91440.732249286768</v>
+        <v>8.965458488928345E-4</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>115344.9690760001</v>
+        <v>1.00309501946005E-3</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>121047.2440269201</v>
+        <v>8.2126850071070369E-4</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>120948.79932970674</v>
+        <v>8.4976747618045224E-4</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>117383.29215263342</v>
+        <v>7.1182262426147962E-4</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>123127.10862456677</v>
+        <v>1.7123790270281364E-3</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>114725.79836802675</v>
+        <v>9.6987339781522217E-4</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>124562.44907814678</v>
+        <v>2.4388672270152779E-4</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>137433.65962103344</v>
+        <v>5.2354989170099104E-4</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>145122.43462956007</v>
+        <v>6.7428267983028159E-4</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>128143.43887404009</v>
+        <v>1.4431821031760845E-3</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>126318.60358468677</v>
+        <v>9.4843014424602788E-4</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>107828.50338752674</v>
+        <v>1.6871179318508666E-3</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>94326.918991453422</v>
+        <v>4.2023128324493843E-3</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>74851.04301986011</v>
+        <v>2.5460810058365747E-3</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>92600.108400646757</v>
+        <v>1.1853097369434109E-3</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>117711.08091633343</v>
+        <v>6.2372065724712589E-4</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>147913.4492156468</v>
+        <v>5.2990435089861918E-4</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>140435.08477254008</v>
+        <v>1.4372644469542418E-3</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>130827.90323600678</v>
+        <v>1.2101018152949538E-3</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>150454.44263618012</v>
+        <v>6.3029842014447612E-4</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>173407.90690484678</v>
+        <v>6.8497720158950922E-4</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>175964.84634857342</v>
+        <v>5.9556829622860229E-4</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>177024.22768584677</v>
+        <v>8.3562150418276416E-4</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>191851.02490282012</v>
+        <v>9.680136148033895E-4</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>180826.01983911343</v>
+        <v>2.2181132591011909E-3</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>160982.12480948013</v>
+        <v>2.7700774771650346E-3</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>161802.8674381134</v>
+        <v>3.5598733666413513E-3</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>119508.6983888001</v>
+        <v>4.3323486018964309E-3</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>122100.31699476676</v>
+        <v>2.4618269888064931E-3</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>91304.551704486774</v>
+        <v>4.8426034627692899E-3</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>58489.850016440083</v>
+        <v>7.7490711264074598E-3</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>64051.255196966762</v>
+        <v>4.1636420124058693E-3</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>99676.98059210011</v>
+        <v>2.6514007600237561E-3</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>111976.64493171342</v>
+        <v>2.0745355939400388E-3</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>103504.2131481401</v>
+        <v>2.6078900675972952E-3</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>124227.40669344676</v>
+        <v>2.1434207625002253E-3</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>148238.11812183345</v>
+        <v>1.6364047729634146E-3</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>155961.48826458005</v>
+        <v>1.108368577493366E-3</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>148105.45759641341</v>
+        <v>1.9013670752669038E-3</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>150907.89714724012</v>
+        <v>8.6145923926999723E-4</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>141654.38974160678</v>
+        <v>1.0084539633395827E-3</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>139406.97865666013</v>
+        <v>1.0850663918571912E-3</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>123574.46659566676</v>
+        <v>1.1187537214118984E-3</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>109826.17391929343</v>
+        <v>8.6305963764600339E-4</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>121642.37181319341</v>
+        <v>1.6225534186028352E-3</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>143619.0175474734</v>
+        <v>1.4705356921121855E-3</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>140017.49243220012</v>
+        <v>2.5833873771890139E-3</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>131137.06319406012</v>
+        <v>1.570819839153436E-3</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>145925.54695623345</v>
+        <v>1.4536004303530843E-3</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>158533.16287451348</v>
+        <v>8.4234256842483362E-4</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>159694.14306631344</v>
+        <v>2.495891968662975E-3</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>177593.36258654014</v>
+        <v>2.847860941657347E-3</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>158109.69985760676</v>
+        <v>4.2574737486094031E-3</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>216616.47398479344</v>
+        <v>2.18761307757072E-3</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>257861.57009445364</v>
+        <v>3.579949782110296E-3</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>263816.35934734694</v>
+        <v>2.6471985738527278E-3</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>273829.19441770698</v>
+        <v>2.5763585095820722E-3</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>268594.74803384702</v>
+        <v>2.1070205498655466E-3</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>218193.51322093341</v>
+        <v>3.2408783763201981E-3</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>205788.76264662013</v>
+        <v>2.7226809729523857E-3</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>196105.51349490011</v>
+        <v>1.5948317482815302E-3</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>179601.82835518676</v>
+        <v>3.4167167093643821E-3</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>267815.99570869358</v>
+        <v>7.774580639237136E-3</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>321151.91754067369</v>
+        <v>5.1197699069689935E-3</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>407384.31998911378</v>
+        <v>2.3104465190040332E-3</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>457627.98676594713</v>
+        <v>2.6684930384724783E-3</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>452457.78905583377</v>
+        <v>1.6743018111986861E-3</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>422916.97077879362</v>
+        <v>2.1425067603550283E-3</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>405344.18479953363</v>
+        <v>2.1547641290578356E-3</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>405361.70332145365</v>
+        <v>2.4665145196705002E-3</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>446372.93359686714</v>
+        <v>1.9873948793710234E-3</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>470717.54689648043</v>
+        <v>2.277851887085599E-3</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>556981.28901652712</v>
+        <v>1.0529374971031079E-3</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>611928.59912364709</v>
+        <v>1.3571351458637252E-3</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>590647.3456911071</v>
+        <v>1.6113921656981222E-3</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>747415.84431556042</v>
+        <v>2.4921923937726662E-3</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>971960.78039294027</v>
+        <v>2.8618122198536371E-3</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>1047997.4518073738</v>
+        <v>3.1657542961949152E-3</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>1001720.5892851135</v>
+        <v>3.3279392756539131E-3</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>1214704.7709419744</v>
+        <v>2.9908875524988859E-3</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>1505502.0992105154</v>
+        <v>5.1720687750030827E-3</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>1827598.3978061147</v>
+        <v>1.9872543072648957E-3</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>1433327.2721310479</v>
+        <v>5.0476929805895333E-2</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>1074734.9773931142</v>
+        <v>1.1721819844116304E-2</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>1223390.7379025747</v>
+        <v>4.222799013152193E-3</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>1304498.5465758082</v>
+        <v>3.9258394077221516E-3</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>1308817.9723925479</v>
+        <v>3.010712607531676E-3</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>1401779.5571320278</v>
+        <v>1.8655130280838372E-3</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>1678104.9624722546</v>
+        <v>2.2109433821864317E-3</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>2088484.460492528</v>
+        <v>2.3925094670996885E-3</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>2157084.1740630148</v>
+        <v>5.3668018519864476E-3</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>2025948.7729956545</v>
+        <v>2.9679767242757932E-3</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>2169665.6883531082</v>
+        <v>2.0597910283127346E-3</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>2292052.1453455817</v>
+        <v>4.4861369262481042E-3</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>1751326.2082870549</v>
+        <v>4.8051763789339627E-3</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>2008629.7804241276</v>
+        <v>3.8003445120803393E-3</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>2650371.9407845084</v>
+        <v>3.4482026552117456E-3</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>2726973.059682908</v>
+        <v>2.5767812848429381E-3</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>2741189.2382248682</v>
+        <v>2.4226915627670507E-3</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>2981460.6531414278</v>
+        <v>2.2404075397734354E-3</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>3096884.0845135488</v>
+        <v>1.6911201148894041E-3</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>3255034.1530543617</v>
+        <v>1.1347068323259517E-3</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>3225823.8753971881</v>
+        <v>1.6897368415949795E-3</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>3437523.1960096881</v>
+        <v>9.4001506492031532E-4</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>3758516.027481515</v>
+        <v>1.9464101982215876E-3</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>3879031.8030741885</v>
+        <v>9.6236042178381523E-4</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>3974460.8443210018</v>
+        <v>7.8850019732536105E-4</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>4056973.822277721</v>
+        <v>1.1518798367335342E-3</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>3843548.2690257747</v>
+        <v>2.0441533705873138E-3</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>4014544.9514459353</v>
+        <v>1.1284646268731665E-3</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>4000855.6920753415</v>
+        <v>1.5128480188415022E-3</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>3939366.6586610344</v>
+        <v>8.6857934624994752E-4</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>4927864.3106577033</v>
+        <v>8.8432931198511504E-4</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>5921277.7004628256</v>
+        <v>9.911001464008144E-4</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>6492255.9464338748</v>
+        <v>8.1620610291156836E-4</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>7316842.8939150125</v>
+        <v>2.0291722219110179E-3</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>8217357.9082248183</v>
+        <v>2.444344339496432E-3</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>8366035.2711819401</v>
+        <v>2.0779716624920886E-3</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>9495357.6414239947</v>
+        <v>9.0180864687381746E-4</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>11133042.607667714</v>
+        <v>2.3312255750852994E-3</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>12198217.38722164</v>
+        <v>3.8746893365846475E-3</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>16273749.729628706</v>
+        <v>4.2611833317627917E-3</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>17179034.918953951</v>
+        <v>1.0954584302390146E-2</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>18045825.638148323</v>
+        <v>3.0303199520005622E-3</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>23445463.169361085</v>
+        <v>2.1829465567383493E-3</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>24902817.40827674</v>
+        <v>6.4058624082442249E-3</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>22105156.265544578</v>
+        <v>1.0481822732817912E-2</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>27874737.769493688</v>
+        <v>7.4477287386837373E-3</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>34341930.253048681</v>
+        <v>6.0881011621322307E-3</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>36410577.3195998</v>
+        <v>3.5407818583678996E-3</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>34945654.937674247</v>
+        <v>5.6614661065274531E-3</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>38478329.481789045</v>
+        <v>6.2613683990569062E-3</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>41213057.953724921</v>
+        <v>1.250289613556174E-2</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>43927050.230488382</v>
+        <v>3.7985694328233552E-3</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>38742908.566486292</v>
+        <v>6.6275698903675772E-3</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>32557796.455061015</v>
+        <v>8.7554997856132445E-3</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>29332097.720376134</v>
+        <v>1.1395923625491175E-2</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>29190652.257492919</v>
+        <v>4.2851873614437727E-3</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>21439488.774805989</v>
+        <v>6.7195275924747519E-3</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>23527176.419507679</v>
+        <v>4.1476569206596375E-3</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>24516433.628252525</v>
+        <v>5.7473249291156636E-3</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>17420582.87386952</v>
+        <v>1.5649779121965534E-2</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>14822367.559714446</v>
+        <v>1.6039712477211119E-2</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>14360440.862437204</v>
+        <v>7.4562123044113722E-3</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>15363801.505225407</v>
+        <v>8.0681427420458505E-3</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>19299048.000197191</v>
+        <v>3.9249291339928669E-3</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>20792242.291877154</v>
+        <v>2.8314165389760997E-3</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>23481177.41987649</v>
+        <v>1.9466013508450733E-3</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>24752429.582613338</v>
+        <v>2.4724812813606101E-3</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>24241204.064553972</v>
+        <v>1.9680084348357406E-3</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>25074677.458319467</v>
+        <v>1.6187451095480397E-3</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>26808211.516904324</v>
+        <v>1.4318113097275067E-3</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>27518119.091709763</v>
+        <v>2.8203417902441324E-3</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>29759206.431846593</v>
+        <v>1.257349545681886E-3</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>28902021.745630611</v>
+        <v>1.9864954140841836E-3</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>29981307.463574883</v>
+        <v>1.268347638016219E-3</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>33242157.336769447</v>
+        <v>1.6011310820006127E-3</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>32292253.161854535</v>
+        <v>2.5102723502513457E-3</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>36023994.682891548</v>
+        <v>9.0742495611817377E-4</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>37235058.215001397</v>
+        <v>1.5355815870179527E-3</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>42507043.238862343</v>
+        <v>2.042522798029188E-3</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>45167559.786267698</v>
+        <v>7.0008017959545298E-3</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>44093038.603019737</v>
+        <v>6.1569669388902432E-3</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>37181879.009112842</v>
+        <v>6.1854511705153091E-3</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>36362232.167614408</v>
+        <v>7.7884722905704439E-3</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>33112369.42652281</v>
+        <v>8.0181249798257845E-3</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>20626805.865858782</v>
+        <v>7.8911690026122347E-2</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>13514037.876660405</v>
+        <v>2.7370866093849196E-2</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>13500531.474017054</v>
+        <v>2.1962743824031628E-2</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>18288501.982602853</v>
+        <v>4.5831436077914001E-3</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>22161894.468503136</v>
+        <v>4.0518638654081117E-3</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>22661111.988380324</v>
+        <v>2.6639223535747359E-3</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>26525164.530071396</v>
+        <v>6.2543481795669991E-3</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>23560101.124557238</v>
+        <v>6.6896032812740159E-3</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>26445154.981690485</v>
+        <v>2.3629948687135111E-3</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>30946654.343011577</v>
+        <v>1.1436036280046778E-3</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>34760013.495324127</v>
+        <v>1.9045885194063146E-3</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>32065984.921072826</v>
+        <v>1.8706305471840285E-2</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>28229888.21787101</v>
+        <v>1.286024480893313E-2</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>31834810.451389845</v>
+        <v>3.1169942049278552E-3</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
-        <v>37304425.932496391</v>
+        <v>2.5124970652683873E-3</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>37564115.605087496</v>
+        <v>3.4296408664314325E-3</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>38374748.739929624</v>
+        <v>2.1605041535351778E-3</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>40259458.866779327</v>
+        <v>2.2674225756129729E-3</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>50402985.275884427</v>
+        <v>2.3067904732959857E-3</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>54509618.159026623</v>
+        <v>1.7175846185321201E-3</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>58856710.437953256</v>
+        <v>1.4201598382690753E-3</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>62670790.558874369</v>
+        <v>1.7601826599701858E-3</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257">
-        <v>68917384.102247596</v>
+        <v>1.654220691914228E-3</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>76942028.791497499</v>
+        <v>9.6881563124836796E-4</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>77824471.526648507</v>
+        <v>2.3222342227154549E-3</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>80386169.328607425</v>
+        <v>2.4888959551272057E-3</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>86413197.434657872</v>
+        <v>2.1415696003296929E-3</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>87830787.613459051</v>
+        <v>2.8414047638473192E-3</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>80178770.908502623</v>
+        <v>4.1915457633476157E-3</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>73168316.783447444</v>
+        <v>5.6082310739785637E-3</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>84474936.150665835</v>
+        <v>1.6229045928976016E-3</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>93019984.004199103</v>
+        <v>1.5345860568281708E-3</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>91519006.230577394</v>
+        <v>1.7552590509878196E-3</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>97799123.308421135</v>
+        <v>4.38239562998445E-4</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>113039673.42435606</v>
+        <v>6.4556157621580056E-4</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>122163643.10869908</v>
+        <v>6.4008524440406923E-4</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>128384788.89914244</v>
+        <v>2.6429283672098212E-4</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>139111990.47750708</v>
+        <v>3.8455565008851471E-3</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>145274326.54839864</v>
+        <v>3.3109180573405589E-3</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>138966636.59513828</v>
+        <v>7.8155056074454736E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPFA!!! + other good stuff!
</commit_message>
<xml_diff>
--- a/Code/Data/RVq.xlsx
+++ b/Code/Data/RVq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24735" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28860" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,1372 +346,1372 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0</v>
+        <v>1315.3637977300109</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1375.5980020250099</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>1425.014641360011</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1619.9198181250101</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0</v>
+        <v>1926.8377365500105</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0</v>
+        <v>1986.3859474900109</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0</v>
+        <v>2196.1023644100101</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0</v>
+        <v>2312.9808071350089</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>2405.5867691550088</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0</v>
+        <v>2665.6901069500104</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>2819.7811472300114</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0</v>
+        <v>2805.8586859450079</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0</v>
+        <v>2964.8979311550083</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0</v>
+        <v>2777.0499242100091</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0</v>
+        <v>2548.0467754350093</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>2503.5206714350097</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0</v>
+        <v>3468.1269511050091</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0</v>
+        <v>4339.4259869300095</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0</v>
+        <v>5499.5259629100137</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0</v>
+        <v>7528.0312828800306</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>9570.5049093400303</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>11614.588891255029</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0</v>
+        <v>15025.270876400029</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>16377.291042065028</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0</v>
+        <v>19006.109485130029</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0</v>
+        <v>20914.083867520036</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0</v>
+        <v>20924.033470100028</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0</v>
+        <v>18734.253656015022</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>17184.788341090021</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0</v>
+        <v>20610.877589360032</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0</v>
+        <v>18266.72881409504</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0</v>
+        <v>13139.173335015033</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0</v>
+        <v>13626.299231475032</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0</v>
+        <v>16906.128694870029</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0</v>
+        <v>22269.965064940028</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>27785.777055220031</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0</v>
+        <v>32502.896173050023</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0</v>
+        <v>37158.537380790018</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0</v>
+        <v>36503.846555610027</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0</v>
+        <v>35040.304537130025</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0</v>
+        <v>32755.21897145002</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0</v>
+        <v>32279.002820275025</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>0</v>
+        <v>31256.226655550028</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0</v>
+        <v>32727.204127215024</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0</v>
+        <v>44120.455765755061</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0</v>
+        <v>49791.423193930103</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>0</v>
+        <v>52375.271297550091</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>4.3842282610692326E-4</v>
+        <v>58380.366270060113</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5.7635459221792402E-3</v>
+        <v>57424.48306182013</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3.4742413835288353E-3</v>
+        <v>41837.24178740006</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3.423846440254862E-3</v>
+        <v>35249.169725570027</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1.1769097214180059E-3</v>
+        <v>41069.132554650045</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>5.266672963978406E-4</v>
+        <v>50833.653015150099</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>6.0297968775836666E-4</v>
+        <v>58771.032502140108</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1.5322466184284026E-3</v>
+        <v>63736.298642185109</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2.6489129979985644E-4</v>
+        <v>67334.690257965092</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>2.8912988887455242E-4</v>
+        <v>77356.619275930105</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>6.0971688173581744E-4</v>
+        <v>87093.008826900099</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2.9007766401845087E-4</v>
+        <v>91936.752913315097</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>4.4148067889388502E-4</v>
+        <v>93997.819644245101</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3.3081102379655964E-4</v>
+        <v>100592.49228948011</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>1.0325217359824781E-3</v>
+        <v>100045.76856968011</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>3.3849844641362542E-4</v>
+        <v>104222.7292833901</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>4.2932739999858782E-4</v>
+        <v>115852.93517807011</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1.5141453322527389E-3</v>
+        <v>113507.0197978701</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>1.807267658398972E-3</v>
+        <v>100815.26861507009</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>2.3498565942443213E-3</v>
+        <v>83255.818882515101</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>8.965458488928345E-4</v>
+        <v>83285.392983700105</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>1.00309501946005E-3</v>
+        <v>101989.1201327351</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>8.2126850071070369E-4</v>
+        <v>115333.35361103507</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>8.4976747618045224E-4</v>
+        <v>124019.50111495506</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>7.1182262426147962E-4</v>
+        <v>123620.3171383451</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>1.7123790270281364E-3</v>
+        <v>114987.18168241509</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>9.6987339781522217E-4</v>
+        <v>123193.76534830511</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>2.4388672270152779E-4</v>
+        <v>118521.79109252008</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>5.2354989170099104E-4</v>
+        <v>136051.14999493011</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>6.7428267983028159E-4</v>
+        <v>138047.20536421507</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1.4431821031760845E-3</v>
+        <v>141363.61237463009</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>9.4843014424602788E-4</v>
+        <v>126274.87379032013</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>1.6871179318508666E-3</v>
+        <v>120876.11005735009</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>4.2023128324493843E-3</v>
+        <v>103423.8054040701</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>2.5460810058365747E-3</v>
+        <v>81367.113054335103</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1.1853097369434109E-3</v>
+        <v>83409.431207800109</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>6.2372065724712589E-4</v>
+        <v>104307.93901395009</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>5.2990435089861918E-4</v>
+        <v>135181.18188520512</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1.4372644469542418E-3</v>
+        <v>143249.14798396011</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>1.2101018152949538E-3</v>
+        <v>135659.87270285009</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>6.3029842014447612E-4</v>
+        <v>137451.79323821509</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>6.8497720158950922E-4</v>
+        <v>162122.75175617012</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>5.9556829622860229E-4</v>
+        <v>168333.24966779008</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>8.3562150418276416E-4</v>
+        <v>174221.81873573514</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>9.680136148033895E-4</v>
+        <v>191680.9298217551</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>2.2181132591011909E-3</v>
+        <v>188120.37860241509</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>2.7700774771650346E-3</v>
+        <v>165931.17673565011</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>3.5598733666413513E-3</v>
+        <v>165636.92181192507</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>4.3323486018964309E-3</v>
+        <v>148006.3869118251</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>2.4618269888064931E-3</v>
+        <v>123230.6615817001</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>4.8426034627692899E-3</v>
+        <v>107720.51487026509</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>7.7490711264074598E-3</v>
+        <v>70909.479977950105</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>4.1636420124058693E-3</v>
+        <v>60247.762770475092</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>2.6514007600237561E-3</v>
+        <v>81896.879837770102</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>2.0745355939400388E-3</v>
+        <v>112490.76285060009</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>2.6078900675972952E-3</v>
+        <v>106823.3617819301</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>2.1434207625002253E-3</v>
+        <v>113931.0866610551</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>1.6364047729634146E-3</v>
+        <v>141580.29311559509</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>1.108368577493366E-3</v>
+        <v>148324.8257093601</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>1.9013670752669038E-3</v>
+        <v>154315.71915964509</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>8.6145923926999723E-4</v>
+        <v>150586.97080100508</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>1.0084539633395827E-3</v>
+        <v>143694.88673032509</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>1.0850663918571912E-3</v>
+        <v>134664.01147340011</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>1.1187537214118984E-3</v>
+        <v>129435.54201876512</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>8.6305963764600339E-4</v>
+        <v>118432.41188593009</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1.6225534186028352E-3</v>
+        <v>107861.87951621009</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1.4705356921121855E-3</v>
+        <v>128805.52144809507</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>2.5833873771890139E-3</v>
+        <v>146580.83985197011</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1.570819839153436E-3</v>
+        <v>136004.1357543701</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>1.4536004303530843E-3</v>
+        <v>140010.21044837509</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>8.4234256842483362E-4</v>
+        <v>146182.74103980511</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>2.495891968662975E-3</v>
+        <v>163701.89167999011</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>2.847860941657347E-3</v>
+        <v>167942.63915129012</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>4.2574737486094031E-3</v>
+        <v>169711.80120095512</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>2.18761307757072E-3</v>
+        <v>184502.8838450851</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>3.579949782110296E-3</v>
+        <v>245688.32837225019</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>2.6471985738527278E-3</v>
+        <v>271965.04911012028</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>2.5763585095820722E-3</v>
+        <v>266740.93921902531</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>2.1070205498655466E-3</v>
+        <v>271036.76269612531</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>3.2408783763201981E-3</v>
+        <v>238101.87112852017</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>2.7226809729523857E-3</v>
+        <v>220236.1945018401</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>1.5948317482815302E-3</v>
+        <v>192210.58568237509</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>3.4167167093643821E-3</v>
+        <v>186829.27406330511</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>7.774580639237136E-3</v>
+        <v>212768.13884244015</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>5.1197699069689935E-3</v>
+        <v>305939.29106990539</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>2.3104465190040332E-3</v>
+        <v>356717.59235425037</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>2.6684930384724783E-3</v>
+        <v>429878.89634837548</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>1.6743018111986861E-3</v>
+        <v>451595.51117691537</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>2.1425067603550283E-3</v>
+        <v>448282.82561007031</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>2.1547641290578356E-3</v>
+        <v>407371.64746339031</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>2.4665145196705002E-3</v>
+        <v>383370.09196791536</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>1.9873948793710234E-3</v>
+        <v>432542.80403643043</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>2.277851887085599E-3</v>
+        <v>463997.88949030545</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>1.0529374971031079E-3</v>
+        <v>516911.6574055854</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>1.3571351458637252E-3</v>
+        <v>589334.01239091041</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>1.6113921656981222E-3</v>
+        <v>602774.57311771042</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>2.4921923937726662E-3</v>
+        <v>689612.99377810536</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>2.8618122198536371E-3</v>
+        <v>858831.94657730544</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>3.1657542961949152E-3</v>
+        <v>1030242.4127077354</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>3.3279392756539131E-3</v>
+        <v>1036642.3014031255</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>2.9908875524988859E-3</v>
+        <v>1097202.5595667404</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>5.1720687750030827E-3</v>
+        <v>1400227.0948640015</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>1.9872543072648957E-3</v>
+        <v>1608587.7672443914</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>5.0476929805895333E-2</v>
+        <v>1765280.2528135069</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>1.1721819844116304E-2</v>
+        <v>1143274.4999376158</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>4.222799013152193E-3</v>
+        <v>1169169.6019410314</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>3.9258394077221516E-3</v>
+        <v>1217597.9275156313</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>3.010712607531676E-3</v>
+        <v>1293817.9891333862</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>1.8655130280838372E-3</v>
+        <v>1366364.1867408312</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>2.2109433821864317E-3</v>
+        <v>1502820.8831636913</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>2.3925094670996885E-3</v>
+        <v>1824239.2267509415</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>5.3668018519864476E-3</v>
+        <v>2163285.3354281113</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>2.9679767242757932E-3</v>
+        <v>2172309.9831751613</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>2.0597910283127346E-3</v>
+        <v>2032361.0599833715</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>4.4861369262481042E-3</v>
+        <v>2262380.1158363163</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>4.8051763789339627E-3</v>
+        <v>1993155.3825385717</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>3.8003445120803393E-3</v>
+        <v>1875158.905676251</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>3.4482026552117456E-3</v>
+        <v>2344261.0807408318</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>2.5767812848429381E-3</v>
+        <v>2699069.4391696565</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>2.4226915627670507E-3</v>
+        <v>2828864.8159628217</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>2.2404075397734354E-3</v>
+        <v>2931934.3581887963</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>1.6911201148894041E-3</v>
+        <v>3108008.0696862866</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>1.1347068323259517E-3</v>
+        <v>3159575.104091302</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>1.6897368415949795E-3</v>
+        <v>3263443.1613739766</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>9.4001506492031532E-4</v>
+        <v>3365203.6281479714</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>1.9464101982215876E-3</v>
+        <v>3597192.0822347319</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>9.6236042178381523E-4</v>
+        <v>3684865.2019937066</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>7.8850019732536105E-4</v>
+        <v>3909493.7693313467</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>1.1518798367335342E-3</v>
+        <v>4105703.7921629418</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>2.0441533705873138E-3</v>
+        <v>3919031.2387455311</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>1.1284646268731665E-3</v>
+        <v>3688721.1928033014</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>1.5128480188415022E-3</v>
+        <v>4010677.8216021764</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>8.6857934624994752E-4</v>
+        <v>3960019.0482852366</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>8.8432931198511504E-4</v>
+        <v>4327753.6742958222</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>9.911001464008144E-4</v>
+        <v>5269758.8085020641</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>8.1620610291156836E-4</v>
+        <v>6192346.0050251167</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>2.0291722219110179E-3</v>
+        <v>6943430.0881967368</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>2.444344339496432E-3</v>
+        <v>7762049.23469349</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>2.0779716624920886E-3</v>
+        <v>8253222.9797381163</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>9.0180864687381746E-4</v>
+        <v>8901316.0385081861</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>2.3312255750852994E-3</v>
+        <v>10647205.260520577</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>3.8746893365846475E-3</v>
+        <v>11509632.502190247</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>4.2611833317627917E-3</v>
+        <v>14348497.126580616</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>1.0954584302390146E-2</v>
+        <v>17537085.246482797</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>3.0303199520005622E-3</v>
+        <v>17585695.030689467</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>2.1829465567383493E-3</v>
+        <v>20756946.40742423</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>6.4058624082442249E-3</v>
+        <v>24763204.620472927</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>1.0481822732817912E-2</v>
+        <v>22900698.408262745</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>7.4477287386837373E-3</v>
+        <v>25607272.334110003</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>6.0881011621322307E-3</v>
+        <v>31203506.870986912</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>3.5407818583678996E-3</v>
+        <v>35203793.055877283</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>5.6614661065274531E-3</v>
+        <v>35043057.684633344</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>6.2613683990569062E-3</v>
+        <v>37644355.532301262</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>1.250289613556174E-2</v>
+        <v>38978619.186572649</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>3.7985694328233552E-3</v>
+        <v>40722966.372506499</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>6.6275698903675772E-3</v>
+        <v>41813244.566358671</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>8.7554997856132445E-3</v>
+        <v>36048900.506774016</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>1.1395923625491175E-2</v>
+        <v>29925427.406741865</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>4.2851873614437727E-3</v>
+        <v>29331497.835340779</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>6.7195275924747519E-3</v>
+        <v>24290282.186877981</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>4.1476569206596375E-3</v>
+        <v>24785793.070038088</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>5.7473249291156636E-3</v>
+        <v>24047766.204866022</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>1.5649779121965534E-2</v>
+        <v>21058942.790233184</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>1.6039712477211119E-2</v>
+        <v>15659823.022392951</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>7.4562123044113722E-3</v>
+        <v>15414756.34681794</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>8.0681427420458505E-3</v>
+        <v>14170010.369014464</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>3.9249291339928669E-3</v>
+        <v>17808898.583987959</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>2.8314165389760997E-3</v>
+        <v>20521965.192191098</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>1.9466013508450733E-3</v>
+        <v>22440150.281908877</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>2.4724812813606101E-3</v>
+        <v>24615925.490032535</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>1.9680084348357406E-3</v>
+        <v>23983078.074048109</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>1.6187451095480397E-3</v>
+        <v>24068423.822501879</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>1.4318113097275067E-3</v>
+        <v>26516724.282401368</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>2.8203417902441324E-3</v>
+        <v>26634135.021752536</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>1.257349545681886E-3</v>
+        <v>27649975.651553161</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>1.9864954140841836E-3</v>
+        <v>29126914.239670467</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>1.268347638016219E-3</v>
+        <v>29692994.036778968</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>1.6011310820006127E-3</v>
+        <v>31137825.888302848</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>2.5102723502513457E-3</v>
+        <v>31296045.825414576</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>9.0742495611817377E-4</v>
+        <v>33795239.657185391</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>1.5355815870179527E-3</v>
+        <v>37707344.163359694</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>2.042522798029188E-3</v>
+        <v>38725072.557708845</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>7.0008017959545298E-3</v>
+        <v>44244652.148285955</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>6.1569669388902432E-3</v>
+        <v>45299261.988479927</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>6.1854511705153091E-3</v>
+        <v>42604395.066828199</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>7.7884722905704439E-3</v>
+        <v>35372290.71928928</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>8.0181249798257845E-3</v>
+        <v>36067267.459674887</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>7.8911690026122347E-2</v>
+        <v>28175161.622374009</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>2.7370866093849196E-2</v>
+        <v>15610553.037969176</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>2.1962743824031628E-2</v>
+        <v>12590840.708929366</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>4.5831436077914001E-3</v>
+        <v>16000374.982121006</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>4.0518638654081117E-3</v>
+        <v>20499311.933842886</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>2.6639223535747359E-3</v>
+        <v>23105456.602027714</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>6.2543481795669991E-3</v>
+        <v>24797597.954079892</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>6.6896032812740159E-3</v>
+        <v>24444081.258600011</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>2.3629948687135111E-3</v>
+        <v>24494882.209248796</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>1.1436036280046778E-3</v>
+        <v>29217571.215604752</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>1.9045885194063146E-3</v>
+        <v>32652641.509396587</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>1.8706305471840285E-2</v>
+        <v>33530997.202157315</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>1.286024480893313E-2</v>
+        <v>29414538.203635938</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>3.1169942049278552E-3</v>
+        <v>29863926.754086852</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
-        <v>2.5124970652683873E-3</v>
+        <v>35142493.08107882</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>3.4296408664314325E-3</v>
+        <v>35658877.658374175</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>2.1605041535351778E-3</v>
+        <v>38907722.715940475</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>2.2674225756129729E-3</v>
+        <v>39709883.821450263</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>2.3067904732959857E-3</v>
+        <v>44718352.785054527</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>1.7175846185321201E-3</v>
+        <v>53140762.304331213</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>1.4201598382690753E-3</v>
+        <v>57977427.747817166</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>1.7601826599701858E-3</v>
+        <v>63182473.760348663</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257">
-        <v>1.654220691914228E-3</v>
+        <v>65079005.009355068</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>9.6881563124836796E-4</v>
+        <v>73372872.698395833</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>2.3222342227154549E-3</v>
+        <v>78852100.137022942</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>2.4888959551272057E-3</v>
+        <v>79831420.615203455</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>2.1415696003296929E-3</v>
+        <v>82409603.634208873</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>2.8414047638473192E-3</v>
+        <v>87932142.909446791</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>4.1915457633476157E-3</v>
+        <v>82985786.766690925</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>5.6082310739785637E-3</v>
+        <v>79459616.660862401</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>1.6229045928976016E-3</v>
+        <v>75488105.208436862</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>1.5345860568281708E-3</v>
+        <v>86260105.092857435</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>1.7552590509878196E-3</v>
+        <v>92810748.56076172</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>4.38239562998445E-4</v>
+        <v>94913751.338819668</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>6.4556157621580056E-4</v>
+        <v>103455361.91647168</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>6.4008524440406923E-4</v>
+        <v>113355637.27409409</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>2.6429283672098212E-4</v>
+        <v>123991799.2613039</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>3.8455565008851471E-3</v>
+        <v>139075630.59178457</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>3.3109180573405589E-3</v>
+        <v>142021215.76818734</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>7.8155056074454736E-4</v>
+        <v>148959689.47722089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>